<commit_message>
se modif los DataSources
</commit_message>
<xml_diff>
--- a/Smoke/DataSource - Emision AP No Enlatada.xlsx
+++ b/Smoke/DataSource - Emision AP No Enlatada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E66C0D6-3E3C-471C-8220-BBE9BE44B5CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780347AD-122B-406D-8652-0FBA257F1816}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,13 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="41">
-  <si>
-    <t>Usuario</t>
-  </si>
-  <si>
-    <t>Contrasenia</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="37">
   <si>
     <t>NroCuenta</t>
   </si>
@@ -103,12 +97,6 @@
   </si>
   <si>
     <t>D.N.I.</t>
-  </si>
-  <si>
-    <t>Ambiente</t>
-  </si>
-  <si>
-    <t>URL</t>
   </si>
   <si>
     <t>Tarjeta de Crédito</t>
@@ -271,7 +259,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -287,8 +275,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -375,7 +361,7 @@
       <sheetData sheetId="3">
         <row r="2">
           <cell r="A2">
-            <v>21840813</v>
+            <v>21840815</v>
           </cell>
         </row>
       </sheetData>
@@ -647,42 +633,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -691,127 +675,95 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="L1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="O1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R1" t="s">
+    </row>
+    <row r="2" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="D2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="S1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="14"/>
-      <c r="H2" s="13" t="s">
+      <c r="E2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="13" t="s">
+      <c r="K2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="11">
+        <v>1</v>
+      </c>
+      <c r="N2" s="11">
+        <v>400000</v>
+      </c>
+      <c r="O2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" s="13">
-        <v>1</v>
-      </c>
-      <c r="R2" s="13">
-        <v>400000</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="T2" s="13">
+      <c r="P2" s="11">
         <f>[1]DatosAP!$A$2</f>
-        <v>21840813</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="E15" s="1"/>
+        <v>21840815</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{AF45BEF6-27B9-4633-AA27-4FF92CC3A288}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -828,43 +780,43 @@
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E1" s="6">
         <v>6328381177</v>
       </c>
       <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
         <v>18</v>
-      </c>
-      <c r="N1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" t="s">
-        <v>20</v>
       </c>
       <c r="Q1">
         <v>1</v>
@@ -873,7 +825,7 @@
         <v>150000</v>
       </c>
       <c r="S1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="T1">
         <v>21840807</v>
@@ -881,43 +833,43 @@
     </row>
     <row r="2" spans="1:20" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E2" s="10">
         <v>5944603681</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="7" t="s">
+      <c r="O2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="Q2" s="7">
         <v>1</v>
@@ -926,7 +878,7 @@
         <v>400000</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="T2" s="7">
         <v>21840805</v>
@@ -934,43 +886,43 @@
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E3" s="3">
         <v>7557632631</v>
       </c>
       <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" t="s">
         <v>15</v>
       </c>
-      <c r="I3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" t="s">
         <v>18</v>
-      </c>
-      <c r="N3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" t="s">
-        <v>16</v>
-      </c>
-      <c r="P3" t="s">
-        <v>20</v>
       </c>
       <c r="Q3">
         <v>1</v>
@@ -979,7 +931,7 @@
         <v>400000</v>
       </c>
       <c r="S3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="T3">
         <v>21840806</v>
@@ -987,16 +939,16 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E6" s="5">
         <v>9651159553</v>
@@ -1005,31 +957,31 @@
         <v>2302</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" t="s">
         <v>15</v>
       </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" t="s">
-        <v>18</v>
-      </c>
-      <c r="N6" t="s">
-        <v>17</v>
-      </c>
       <c r="O6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="Q6">
         <v>1</v>
@@ -1038,7 +990,7 @@
         <v>550000</v>
       </c>
       <c r="S6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="T6">
         <v>21840810</v>
@@ -1046,16 +998,16 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E7" s="5">
         <v>9651159553</v>
@@ -1064,31 +1016,31 @@
         <v>2302</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" t="s">
         <v>15</v>
       </c>
-      <c r="I7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" t="s">
-        <v>18</v>
-      </c>
-      <c r="N7" t="s">
-        <v>17</v>
-      </c>
       <c r="O7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="Q7">
         <v>1</v>
@@ -1097,7 +1049,7 @@
         <v>550000</v>
       </c>
       <c r="S7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="T7">
         <v>21840811</v>
@@ -1105,16 +1057,16 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E8" s="5">
         <v>9651159553</v>
@@ -1123,31 +1075,31 @@
         <v>2302</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" t="s">
         <v>15</v>
       </c>
-      <c r="I8" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" t="s">
-        <v>18</v>
-      </c>
-      <c r="N8" t="s">
-        <v>17</v>
-      </c>
       <c r="O8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="Q8">
         <v>1</v>
@@ -1156,7 +1108,7 @@
         <v>550000</v>
       </c>
       <c r="S8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="T8">
         <v>21840812</v>
@@ -1164,16 +1116,16 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E9" s="5">
         <v>9651159553</v>
@@ -1182,31 +1134,31 @@
         <v>2302</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" t="s">
+        <v>16</v>
+      </c>
+      <c r="N9" t="s">
         <v>15</v>
       </c>
-      <c r="I9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N9" t="s">
-        <v>17</v>
-      </c>
       <c r="O9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="Q9">
         <v>1</v>
@@ -1215,7 +1167,7 @@
         <v>550000</v>
       </c>
       <c r="S9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="T9">
         <v>21840813</v>
@@ -1223,16 +1175,16 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E10" s="5">
         <v>9651159553</v>
@@ -1241,31 +1193,31 @@
         <v>2302</v>
       </c>
       <c r="G10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" t="s">
         <v>15</v>
       </c>
-      <c r="I10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J10" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" t="s">
-        <v>18</v>
-      </c>
-      <c r="N10" t="s">
-        <v>17</v>
-      </c>
       <c r="O10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="Q10">
         <v>1</v>
@@ -1274,7 +1226,7 @@
         <v>550000</v>
       </c>
       <c r="S10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="T10">
         <v>21840814</v>
@@ -1282,16 +1234,16 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E11" s="5">
         <v>9651159553</v>
@@ -1300,31 +1252,31 @@
         <v>2302</v>
       </c>
       <c r="G11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N11" t="s">
         <v>15</v>
       </c>
-      <c r="I11" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" t="s">
-        <v>18</v>
-      </c>
-      <c r="N11" t="s">
-        <v>17</v>
-      </c>
       <c r="O11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="Q11">
         <v>1</v>
@@ -1333,7 +1285,7 @@
         <v>550000</v>
       </c>
       <c r="S11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="T11">
         <v>21840815</v>
@@ -1341,16 +1293,16 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E12" s="5">
         <v>9651159553</v>
@@ -1359,31 +1311,31 @@
         <v>2302</v>
       </c>
       <c r="G12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" t="s">
+        <v>16</v>
+      </c>
+      <c r="N12" t="s">
         <v>15</v>
       </c>
-      <c r="I12" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" t="s">
-        <v>16</v>
-      </c>
-      <c r="L12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12" t="s">
-        <v>18</v>
-      </c>
-      <c r="N12" t="s">
-        <v>17</v>
-      </c>
       <c r="O12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="Q12">
         <v>1</v>
@@ -1392,7 +1344,7 @@
         <v>550000</v>
       </c>
       <c r="S12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="T12">
         <v>21840816</v>
@@ -1400,16 +1352,16 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E13" s="5">
         <v>9651159553</v>
@@ -1418,31 +1370,31 @@
         <v>2302</v>
       </c>
       <c r="G13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" t="s">
+        <v>17</v>
+      </c>
+      <c r="M13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N13" t="s">
         <v>15</v>
       </c>
-      <c r="I13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" t="s">
-        <v>16</v>
-      </c>
-      <c r="L13" t="s">
-        <v>19</v>
-      </c>
-      <c r="M13" t="s">
-        <v>18</v>
-      </c>
-      <c r="N13" t="s">
-        <v>17</v>
-      </c>
       <c r="O13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="Q13">
         <v>1</v>
@@ -1451,7 +1403,7 @@
         <v>550000</v>
       </c>
       <c r="S13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="T13">
         <v>21840817</v>
@@ -1459,16 +1411,16 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E14" s="5">
         <v>9651159553</v>
@@ -1477,31 +1429,31 @@
         <v>2302</v>
       </c>
       <c r="G14" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" t="s">
+        <v>16</v>
+      </c>
+      <c r="N14" t="s">
         <v>15</v>
       </c>
-      <c r="I14" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" t="s">
-        <v>16</v>
-      </c>
-      <c r="L14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M14" t="s">
-        <v>18</v>
-      </c>
-      <c r="N14" t="s">
-        <v>17</v>
-      </c>
       <c r="O14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="Q14">
         <v>1</v>
@@ -1510,7 +1462,7 @@
         <v>550000</v>
       </c>
       <c r="S14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="T14">
         <v>21840818</v>

</xml_diff>